<commit_message>
updated document sample import files
</commit_message>
<xml_diff>
--- a/public/files/import/invoices.xlsx
+++ b/public/files/import/invoices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="13620" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="invoices" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>invoice_number</t>
   </si>
@@ -39,6 +39,12 @@
     <t>amount</t>
   </si>
   <si>
+    <t>discount_type</t>
+  </si>
+  <si>
+    <t>discount_rate</t>
+  </si>
+  <si>
     <t>currency_code</t>
   </si>
   <si>
@@ -87,6 +93,9 @@
     <t>paid</t>
   </si>
   <si>
+    <t>percentage</t>
+  </si>
+  <si>
     <t>USD</t>
   </si>
   <si>
@@ -147,7 +156,7 @@
     <t>INV-00001 added!</t>
   </si>
   <si>
-    <t>$10.00 Payment</t>
+    <t>$9.00 Payment</t>
   </si>
   <si>
     <t>code</t>
@@ -163,6 +172,12 @@
   </si>
   <si>
     <t>invoices.sub_total</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>invoices.discount</t>
   </si>
   <si>
     <t>invoices.total</t>
@@ -201,12 +216,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,69 +242,108 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,38 +358,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,36 +381,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,37 +395,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,145 +557,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,26 +586,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -625,6 +613,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -640,11 +637,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,170 +686,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -857,63 +865,65 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1211,35 +1221,37 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="H1" sqref="H$1:H$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="17.0092592592593" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.0092592592593" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.00925925925926" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.0092592592593" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.0092592592593" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.00925925925926" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.0092592592593" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.0092592592593" style="3" customWidth="1"/>
-    <col min="9" max="10" width="16.0092592592593" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.0092592592593" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.0092592592593" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.0092592592593" style="1" customWidth="1"/>
-    <col min="14" max="15" width="18.0092592592593" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.0092592592593" style="1" customWidth="1"/>
-    <col min="17" max="17" width="19.0092592592593" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.0092592592593" style="1" customWidth="1"/>
-    <col min="19" max="19" width="6.00925925925926" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.00925925925926" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.0078125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.0078125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.0078125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.0078125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.0078125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.0078125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="12.4375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="16.0078125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.0078125" style="3" customWidth="1"/>
+    <col min="11" max="12" width="16.0078125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="29.0078125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="22.0078125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.0078125" style="1" customWidth="1"/>
+    <col min="16" max="17" width="18.0078125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.0078125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="19.0078125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.0078125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6.0078125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="8.0078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" spans="1:20">
+    <row r="1" ht="18.75" customHeight="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1249,25 +1261,25 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1300,13 +1312,19 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1" spans="1:19">
+    <row r="2" ht="18.75" customHeight="1" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5">
         <v>43831</v>
@@ -1314,26 +1332,32 @@
       <c r="E2" s="5">
         <v>43831</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="14">
+        <v>9</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="15">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="13">
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="14">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" s="7" t="s">
+      <c r="K2" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1349,19 +1373,19 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="17.0092592592593" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.0092592592593" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.0078125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.0078125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.0092592592593" style="8" customWidth="1"/>
-    <col min="5" max="5" width="10.0092592592593" style="9" customWidth="1"/>
-    <col min="6" max="7" width="6.00925925925926" style="9" customWidth="1"/>
-    <col min="8" max="8" width="4.00925925925926" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.0078125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="10.0078125" style="9" customWidth="1"/>
+    <col min="6" max="7" width="6.0078125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="4.0078125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:8">
@@ -1369,39 +1393,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E2" s="11">
         <v>1</v>
@@ -1430,12 +1454,12 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.0092592592593" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.0092592592593" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.0092592592593" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.00925925925926" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.0078125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.0078125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.0078125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.0078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:4">
@@ -1443,10 +1467,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -1466,15 +1490,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.0092592592593" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.00925925925926" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.00925925925926" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.0092592592593" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.0078125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.0078125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.0078125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.0078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:4">
@@ -1485,34 +1509,34 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1526,19 +1550,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17.0092592592593" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.0092592592593" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.0092592592593" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.00925925925926" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.0092592592593" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.0078125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.0078125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.0078125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.0078125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.0078125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:5">
@@ -1546,27 +1570,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D2" s="6">
         <v>10</v>
@@ -1577,19 +1601,36 @@
     </row>
     <row r="3" ht="18.75" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D3" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E3" s="6">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" ht="18.75" customHeight="1" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="6">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1605,25 +1646,25 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="17.0092592592593" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.0092592592593" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.287037037037" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.00925925925926" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.0092592592593" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.0092592592593" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.0092592592593" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.0092592592593" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.0092592592593" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.0092592592593" style="1" customWidth="1"/>
-    <col min="11" max="11" width="28.0092592592593" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.0092592592593" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.0092592592593" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.0078125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.0078125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.2890625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.0078125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.0078125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.0078125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.0078125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.0078125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.0078125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.0078125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28.0078125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.0078125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.0078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:13">
@@ -1631,73 +1672,73 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C2" s="5">
         <v>43831</v>
       </c>
       <c r="D2" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>

</xml_diff>